<commit_message>
1) correções no processo haoc;
</commit_message>
<xml_diff>
--- a/CoParticipacaoWebService/src/test/resources/cargill/input/201812/CARGILL.NAO-LOCALIZADO.201812.003.xlsx
+++ b/CoParticipacaoWebService/src/test/resources/cargill/input/201812/CARGILL.NAO-LOCALIZADO.201812.003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="00192" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,42 +22,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
   <si>
     <t xml:space="preserve">EMPRESA</t>
   </si>
   <si>
+    <t xml:space="preserve">MATRICULA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENEFICIÁRIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COD VERBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DT ADMISSÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMANDA HOLANDA COSTA BISSONI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANA CAROLINA MOCCI FRANCOSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANALICE SILVA MEIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTHUR LIRA DE LUCENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMILA DE PAULA ALMEIDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLAUDIA APARECIDA DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DANIEL OLIVEIRA SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENISE MARTIN MARQUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABIANA CORREA BISPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISABELLA VICTORIA S LIRA LUCENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOAO CARLOS MEIRA DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JULIA LUZ MELO MONTEIRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JULIANA LOURENCO PINTO CARVALHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KASSANDRA MATTERA RODRIGUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LARISSA CAPALBO VIEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAURA MELO TORRES DE PAULA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUISA  VILAS BOAS DE MELO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIZ ANTONIO ROSSI MARTINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUELA PISOK LOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA EDUARDA OLIVEIRA SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOAH STEIRENSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAFAEL MARQUES PREVIATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROBERTA QUITO MARTINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMMY STEIRENSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERGIO STEIRENSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TATIANA AOKI CAVALCANTI SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEO RODRIGUES BARBOSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALDYVANYA SOUSA DUTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALMIR SILVA DE RESENDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANA VITORIA SILVA VIOTTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABIO HAIDAR VIOTTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICTOR SILVA VIOTTO</t>
+  </si>
+  <si>
     <t xml:space="preserve">MATRICULA EMPRESA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENEFICIÁRIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COD VERBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLANO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DT ADMISSÃO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUISA  VILAS BOAS DE MELO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANALICE SILVA MEIRA DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOAO CARLOS MEIRA DOS SANTOS</t>
   </si>
 </sst>
 </file>
@@ -69,11 +171,12 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,6 +203,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF31363B"/>
+      <name val="Monospace"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -171,7 +281,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,7 +355,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF31363B"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -256,21 +366,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -298,10 +409,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>102837</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>65654654665</v>
+        <v>314440</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>31607099810</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>8</v>
@@ -309,8 +420,8 @@
       <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>43101</v>
@@ -321,19 +432,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>195500</v>
+        <v>95616</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>16648305886</v>
+        <v>5524798960</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="n">
-        <v>1</v>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>43101</v>
@@ -347,18 +458,616 @@
         <v>195500</v>
       </c>
       <c r="C4" s="2" t="n">
+        <v>16648305886</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>308147</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>46273892806</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>200495</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>21763564894</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>223421</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>18384976848</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>66694</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>16396297698</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>308913</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>34899729880</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>193855</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>32763389805</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>308147</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>42216953822</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>195500</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>48959287806</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="n">
+      <c r="D12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>314477</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>50623237890</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>310080</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>5426471410</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>191519</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>46635010874</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>314129</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>309889</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>42962425801</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>102837</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>40008</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>15780375658</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>236315</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>66694</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>16396317630</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>199515</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>54690818851</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>308913</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>50599544805</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>309073</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>40180693832</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>199515</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>199515</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>27278507863</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>204496</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>33489295803</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>282805</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>52479392805</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>196537</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>914636103</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>310293</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>27008170874</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="4" t="n">
         <v>43101</v>
       </c>
     </row>
@@ -378,21 +1087,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,6 +1123,75 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>224375</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>54847765893</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>224375</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>21690940832</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>224375</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>43101</v>
       </c>
     </row>
   </sheetData>
@@ -450,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>

</xml_diff>